<commit_message>
Implemented graphical user interface for different operating modes of the program.
</commit_message>
<xml_diff>
--- a/Структура графического интерфейса программы ScanItEasy.xlsx
+++ b/Структура графического интерфейса программы ScanItEasy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Павел\Documents\Dev\ScanItEasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FECFF0-8BC2-4B1F-A836-A4A5AE589067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC7A59F-4E2D-4342-9ECC-112F8B36CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D42CC184-358F-43B8-A50E-375AA33A9444}"/>
+    <workbookView xWindow="2910" yWindow="435" windowWidth="17520" windowHeight="9600" xr2:uid="{D42CC184-358F-43B8-A50E-375AA33A9444}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>Номер строки</t>
   </si>
@@ -150,9 +150,6 @@
     <t>кнопка "Конвертировать"</t>
   </si>
   <si>
-    <t>кнопка выбора файла "Выберитеp pdf-файл для объединения"</t>
-  </si>
-  <si>
     <t>кнопка "Объединить"</t>
   </si>
   <si>
@@ -169,13 +166,43 @@
   </si>
   <si>
     <t>кнопка "Сжать pdf"</t>
+  </si>
+  <si>
+    <t>Лейбл с информацией об условии запуска сканирования</t>
+  </si>
+  <si>
+    <t>Лейбл с информацией об условии запуска конвертации</t>
+  </si>
+  <si>
+    <t>Лейбл с информацией об условии объединения файлов</t>
+  </si>
+  <si>
+    <t>Лейбл с информацией об условии изменения файлов</t>
+  </si>
+  <si>
+    <t>Лейбл с информацией об условии сжатия файла</t>
+  </si>
+  <si>
+    <t>лейбл "Конвертировать pdf в png"</t>
+  </si>
+  <si>
+    <t>кнопка выбора файла "Выберите pdf-файл для конвертации"</t>
+  </si>
+  <si>
+    <t>Лейбл с информацией об условии конвертации</t>
+  </si>
+  <si>
+    <t>кнопка выбора файла "Выберите pdf-файл для объединения"</t>
+  </si>
+  <si>
+    <t>Лейбл "Если нужны все страницы, не заполняйте это поле"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +221,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -299,10 +333,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,22 +377,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -650,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F87559-AB10-465C-990A-9185C21AAD93}">
-  <dimension ref="A1:AW52"/>
+  <dimension ref="A1:AX52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,46 +709,49 @@
     <col min="6" max="6" width="45.5703125" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>
     <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="50" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
-    <col min="12" max="12" width="46.5703125" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1"/>
-    <col min="14" max="14" width="47.85546875" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="11" width="50" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="13" max="13" width="46.5703125" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="15" max="15" width="47.85546875" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" customWidth="1"/>
+    <col min="17" max="17" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="1"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="2"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
@@ -728,71 +774,72 @@
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
-    </row>
-    <row r="2" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="AX1" s="1"/>
+    </row>
+    <row r="2" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>2</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10">
+      <c r="D2" s="9"/>
+      <c r="E2" s="8">
         <v>3</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="10">
+      <c r="F2" s="9"/>
+      <c r="G2" s="8">
         <v>4</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="10">
+      <c r="H2" s="9"/>
+      <c r="I2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8">
         <v>5</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="10">
+      <c r="K2" s="9"/>
+      <c r="L2" s="8">
         <v>6</v>
       </c>
-      <c r="L2" s="11"/>
-      <c r="M2" s="10">
+      <c r="M2" s="9"/>
+      <c r="N2" s="8">
         <v>7</v>
       </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="2">
+      <c r="O2" s="9"/>
+      <c r="P2" s="8">
         <v>8</v>
       </c>
-      <c r="P2" s="2">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="2">
         <v>10</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>11</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>12</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>13</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>14</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>15</v>
       </c>
-      <c r="W2" s="2">
+      <c r="X2" s="2">
         <v>16</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>17</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <v>18</v>
       </c>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="1"/>
+      <c r="AA2" s="2"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
@@ -815,51 +862,56 @@
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
-    </row>
-    <row r="3" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX2" s="1"/>
+    </row>
+    <row r="3" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="7"/>
+      <c r="N3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="1"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -882,51 +934,56 @@
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
-    </row>
-    <row r="4" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX3" s="1"/>
+    </row>
+    <row r="4" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="7"/>
+      <c r="L4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="7"/>
+      <c r="N4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="1"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -949,51 +1006,56 @@
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
-    </row>
-    <row r="5" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX4" s="1"/>
+    </row>
+    <row r="5" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="1"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -1016,63 +1078,68 @@
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
-    </row>
-    <row r="6" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX5" s="1"/>
+    </row>
+    <row r="6" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="8" t="s">
+      <c r="N6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="8" t="s">
+      <c r="P6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="1"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -1095,51 +1162,56 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
-    </row>
-    <row r="7" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX6" s="1"/>
+    </row>
+    <row r="7" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="13"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="1"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -1162,57 +1234,60 @@
       <c r="AU7" s="1"/>
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
-    </row>
-    <row r="8" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX7" s="1"/>
+    </row>
+    <row r="8" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="12" t="s">
+      <c r="O8" s="7"/>
+      <c r="P8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="1"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
@@ -1235,51 +1310,56 @@
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
-    </row>
-    <row r="9" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX8" s="1"/>
+    </row>
+    <row r="9" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="2">
+        <v>6</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="12" t="s">
+      <c r="O9" s="7"/>
+      <c r="P9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="1"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
@@ -1302,49 +1382,56 @@
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
-    </row>
-    <row r="10" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX9" s="1"/>
+    </row>
+    <row r="10" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="12" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="2">
+        <v>7</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="13"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="1"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
@@ -1367,43 +1454,50 @@
       <c r="AU10" s="1"/>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
-    </row>
-    <row r="11" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX10" s="1"/>
+    </row>
+    <row r="11" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="1"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
@@ -1426,41 +1520,50 @@
       <c r="AU11" s="1"/>
       <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
-    </row>
-    <row r="12" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX11" s="1"/>
+    </row>
+    <row r="12" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="12" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="1"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="2">
+        <v>9</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
@@ -1483,39 +1586,48 @@
       <c r="AU12" s="1"/>
       <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
-    </row>
-    <row r="13" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX12" s="1"/>
+    </row>
+    <row r="13" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="12" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="1"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="2">
+        <v>10</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -1538,39 +1650,48 @@
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
-    </row>
-    <row r="14" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX13" s="1"/>
+    </row>
+    <row r="14" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="12" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="1"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="2">
+        <v>11</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
@@ -1593,39 +1714,48 @@
       <c r="AU14" s="1"/>
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
-    </row>
-    <row r="15" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX14" s="1"/>
+    </row>
+    <row r="15" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="12" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="1"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="2">
+        <v>12</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
@@ -1648,39 +1778,44 @@
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
-    </row>
-    <row r="16" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX15" s="1"/>
+    </row>
+    <row r="16" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="12" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="1"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="2">
+        <v>13</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
@@ -1703,39 +1838,44 @@
       <c r="AU16" s="1"/>
       <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
-    </row>
-    <row r="17" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX16" s="1"/>
+    </row>
+    <row r="17" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="12" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="1"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="2">
+        <v>14</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
@@ -1758,39 +1898,44 @@
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
-    </row>
-    <row r="18" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX17" s="1"/>
+    </row>
+    <row r="18" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="12" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="2">
+        <v>15</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
@@ -1813,39 +1958,44 @@
       <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
-    </row>
-    <row r="19" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX18" s="1"/>
+    </row>
+    <row r="19" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="1"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="2">
+        <v>16</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
@@ -1868,39 +2018,44 @@
       <c r="AU19" s="1"/>
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
-    </row>
-    <row r="20" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX19" s="1"/>
+    </row>
+    <row r="20" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="1"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="2">
+        <v>17</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
@@ -1923,39 +2078,44 @@
       <c r="AU20" s="1"/>
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
-    </row>
-    <row r="21" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX20" s="1"/>
+    </row>
+    <row r="21" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="1"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="2">
+        <v>18</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
@@ -1978,37 +2138,44 @@
       <c r="AU21" s="1"/>
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
-    </row>
-    <row r="22" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX21" s="1"/>
+    </row>
+    <row r="22" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
-      <c r="Z22" s="8"/>
-      <c r="AA22" s="1"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="2">
+        <v>19</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="7"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
@@ -2031,37 +2198,42 @@
       <c r="AU22" s="1"/>
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
-    </row>
-    <row r="23" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX22" s="1"/>
+    </row>
+    <row r="23" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="1"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="2">
+        <v>20</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
@@ -2084,37 +2256,42 @@
       <c r="AU23" s="1"/>
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
-    </row>
-    <row r="24" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX23" s="1"/>
+    </row>
+    <row r="24" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="8"/>
-      <c r="AA24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="2">
+        <v>21</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
@@ -2137,37 +2314,42 @@
       <c r="AU24" s="1"/>
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
-    </row>
-    <row r="25" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX24" s="1"/>
+    </row>
+    <row r="25" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="2">
+        <v>22</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25" s="7"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
@@ -2190,37 +2372,40 @@
       <c r="AU25" s="1"/>
       <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
-    </row>
-    <row r="26" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX25" s="1"/>
+    </row>
+    <row r="26" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-      <c r="W26" s="8"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="1"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="2">
+        <v>23</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
@@ -2243,37 +2428,40 @@
       <c r="AU26" s="1"/>
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
-    </row>
-    <row r="27" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX26" s="1"/>
+    </row>
+    <row r="27" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="1"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="2">
+        <v>24</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
@@ -2296,37 +2484,40 @@
       <c r="AU27" s="1"/>
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
-    </row>
-    <row r="28" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX27" s="1"/>
+    </row>
+    <row r="28" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="8"/>
-      <c r="AA28" s="1"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="2">
+        <v>25</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
@@ -2349,37 +2540,40 @@
       <c r="AU28" s="1"/>
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
-    </row>
-    <row r="29" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX28" s="1"/>
+    </row>
+    <row r="29" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="1"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="2">
+        <v>26</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
@@ -2402,37 +2596,40 @@
       <c r="AU29" s="1"/>
       <c r="AV29" s="1"/>
       <c r="AW29" s="1"/>
-    </row>
-    <row r="30" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX29" s="1"/>
+    </row>
+    <row r="30" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="1"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="2">
+        <v>27</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
@@ -2455,37 +2652,40 @@
       <c r="AU30" s="1"/>
       <c r="AV30" s="1"/>
       <c r="AW30" s="1"/>
-    </row>
-    <row r="31" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX30" s="1"/>
+    </row>
+    <row r="31" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="1"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="2">
+        <v>28</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
@@ -2508,37 +2708,40 @@
       <c r="AU31" s="1"/>
       <c r="AV31" s="1"/>
       <c r="AW31" s="1"/>
-    </row>
-    <row r="32" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX31" s="1"/>
+    </row>
+    <row r="32" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="1"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="2">
+        <v>29</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
@@ -2561,8 +2764,9 @@
       <c r="AU32" s="1"/>
       <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
-    </row>
-    <row r="33" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX32" s="1"/>
+    </row>
+    <row r="33" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2612,8 +2816,9 @@
       <c r="AU33" s="1"/>
       <c r="AV33" s="1"/>
       <c r="AW33" s="1"/>
-    </row>
-    <row r="34" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX33" s="1"/>
+    </row>
+    <row r="34" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2663,8 +2868,9 @@
       <c r="AU34" s="1"/>
       <c r="AV34" s="1"/>
       <c r="AW34" s="1"/>
-    </row>
-    <row r="35" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX34" s="1"/>
+    </row>
+    <row r="35" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2714,8 +2920,9 @@
       <c r="AU35" s="1"/>
       <c r="AV35" s="1"/>
       <c r="AW35" s="1"/>
-    </row>
-    <row r="36" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX35" s="1"/>
+    </row>
+    <row r="36" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2765,8 +2972,9 @@
       <c r="AU36" s="1"/>
       <c r="AV36" s="1"/>
       <c r="AW36" s="1"/>
-    </row>
-    <row r="37" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX36" s="1"/>
+    </row>
+    <row r="37" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2816,8 +3024,9 @@
       <c r="AU37" s="1"/>
       <c r="AV37" s="1"/>
       <c r="AW37" s="1"/>
-    </row>
-    <row r="38" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX37" s="1"/>
+    </row>
+    <row r="38" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2867,8 +3076,9 @@
       <c r="AU38" s="1"/>
       <c r="AV38" s="1"/>
       <c r="AW38" s="1"/>
-    </row>
-    <row r="39" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX38" s="1"/>
+    </row>
+    <row r="39" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2918,8 +3128,9 @@
       <c r="AU39" s="1"/>
       <c r="AV39" s="1"/>
       <c r="AW39" s="1"/>
-    </row>
-    <row r="40" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX39" s="1"/>
+    </row>
+    <row r="40" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2969,8 +3180,9 @@
       <c r="AU40" s="1"/>
       <c r="AV40" s="1"/>
       <c r="AW40" s="1"/>
-    </row>
-    <row r="41" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX40" s="1"/>
+    </row>
+    <row r="41" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3020,8 +3232,9 @@
       <c r="AU41" s="1"/>
       <c r="AV41" s="1"/>
       <c r="AW41" s="1"/>
-    </row>
-    <row r="42" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX41" s="1"/>
+    </row>
+    <row r="42" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3071,8 +3284,9 @@
       <c r="AU42" s="1"/>
       <c r="AV42" s="1"/>
       <c r="AW42" s="1"/>
-    </row>
-    <row r="43" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX42" s="1"/>
+    </row>
+    <row r="43" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3122,8 +3336,9 @@
       <c r="AU43" s="1"/>
       <c r="AV43" s="1"/>
       <c r="AW43" s="1"/>
-    </row>
-    <row r="44" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX43" s="1"/>
+    </row>
+    <row r="44" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3173,8 +3388,9 @@
       <c r="AU44" s="1"/>
       <c r="AV44" s="1"/>
       <c r="AW44" s="1"/>
-    </row>
-    <row r="45" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX44" s="1"/>
+    </row>
+    <row r="45" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3224,8 +3440,9 @@
       <c r="AU45" s="1"/>
       <c r="AV45" s="1"/>
       <c r="AW45" s="1"/>
-    </row>
-    <row r="46" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX45" s="1"/>
+    </row>
+    <row r="46" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3275,8 +3492,9 @@
       <c r="AU46" s="1"/>
       <c r="AV46" s="1"/>
       <c r="AW46" s="1"/>
-    </row>
-    <row r="47" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX46" s="1"/>
+    </row>
+    <row r="47" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3326,8 +3544,9 @@
       <c r="AU47" s="1"/>
       <c r="AV47" s="1"/>
       <c r="AW47" s="1"/>
-    </row>
-    <row r="48" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX47" s="1"/>
+    </row>
+    <row r="48" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3377,8 +3596,9 @@
       <c r="AU48" s="1"/>
       <c r="AV48" s="1"/>
       <c r="AW48" s="1"/>
-    </row>
-    <row r="49" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX48" s="1"/>
+    </row>
+    <row r="49" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3428,8 +3648,9 @@
       <c r="AU49" s="1"/>
       <c r="AV49" s="1"/>
       <c r="AW49" s="1"/>
-    </row>
-    <row r="50" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX49" s="1"/>
+    </row>
+    <row r="50" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3479,8 +3700,9 @@
       <c r="AU50" s="1"/>
       <c r="AV50" s="1"/>
       <c r="AW50" s="1"/>
-    </row>
-    <row r="51" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX50" s="1"/>
+    </row>
+    <row r="51" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3530,8 +3752,9 @@
       <c r="AU51" s="1"/>
       <c r="AV51" s="1"/>
       <c r="AW51" s="1"/>
-    </row>
-    <row r="52" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AX51" s="1"/>
+    </row>
+    <row r="52" spans="1:50" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3581,47 +3804,56 @@
       <c r="AU52" s="1"/>
       <c r="AV52" s="1"/>
       <c r="AW52" s="1"/>
+      <c r="AX52" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
+  <mergeCells count="96">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:Z1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E13:F13"/>
@@ -3631,21 +3863,49 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:Y1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>